<commit_message>
cleaning and archetype data
</commit_message>
<xml_diff>
--- a/data/base_scenario/archetypes/stats_trans.xlsx
+++ b/data/base_scenario/archetypes/stats_trans.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\Archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\data\base_scenario\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7675AED-FB11-41C8-A019-C269B05D6C51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D200CB23-5CA4-4F3D-BEB2-90C682FCE622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,12 +43,6 @@
     <t>f_arch_0</t>
   </si>
   <si>
-    <t>conb_car</t>
-  </si>
-  <si>
-    <t>E_car</t>
-  </si>
-  <si>
     <t>f_arch_1</t>
   </si>
   <si>
@@ -68,6 +62,12 @@
   </si>
   <si>
     <t>f_arch_7</t>
+  </si>
+  <si>
+    <t>PC_petrol</t>
+  </si>
+  <si>
+    <t>PC_electric</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -484,7 +484,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -501,10 +501,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -541,10 +541,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -581,10 +581,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -601,10 +601,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -641,10 +641,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -661,10 +661,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -681,10 +681,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -721,10 +721,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -741,10 +741,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -761,10 +761,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
       </c>
       <c r="C17">
         <v>2</v>

</xml_diff>